<commit_message>
order of answers (wip)
</commit_message>
<xml_diff>
--- a/inst/extdata/questions.xlsx
+++ b/inst/extdata/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joses\Documents\_trabajo\packages\rexer\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE0B93C-210B-40EC-8295-D9B047AEB9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B73DF97-A488-4BD8-AFBC-6747123D0BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>type</t>
   </si>
@@ -51,13 +51,52 @@
     <t>a_3</t>
   </si>
   <si>
-    <t>What is the name of the R function for [[1]]?</t>
-  </si>
-  <si>
-    <t>lm&lt;|&gt;glm&lt;|&gt;glm&lt;|&gt;glm.nb&lt;|&gt;model.matrix&lt;|&gt;coef&lt;|&gt;vcov&lt;|&gt;logLik</t>
-  </si>
-  <si>
-    <t>least-squares regression&lt;|&gt;Poisson regression&lt;|&gt;logistic regression&lt;|&gt;negative binomial regression&lt;|&gt;extracting the regressor matrix from a fitted (generalized) linear model object&lt;|&gt;extracting the estimated coefficients from a fitted (generalized) linear model object&lt;|&gt;extracting the estimated covariance matrix from a fitted (generalized) linear model object&lt;|&gt;extracting the fitted log-likelihood from a fitted (generalized) linear model object</t>
+    <t>What is the three-letter country code (ISO 3166-1 alpha-3) for [[1]]?</t>
+  </si>
+  <si>
+    <t>AGO&lt;|&gt;ALB&lt;|&gt;ARG&lt;|&gt;ARM&lt;|&gt;ATG&lt;|&gt;AUS&lt;|&gt;AUT&lt;|&gt;AZE&lt;|&gt;BDI&lt;|&gt;BEL&lt;|&gt;BEN&lt;|&gt;BFA&lt;|&gt;BGD&lt;|&gt;BGR&lt;|&gt;BHR&lt;|&gt;BHS&lt;|&gt;BIH&lt;|&gt;BLR&lt;|&gt;BLZ&lt;|&gt;BMU&lt;|&gt;BOL&lt;|&gt;BRA&lt;|&gt;BRB&lt;|&gt;BRN&lt;|&gt;BTN&lt;|&gt;BWA&lt;|&gt;CAF&lt;|&gt;CAN&lt;|&gt;CHE&lt;|&gt;CHL&lt;|&gt;CHN&lt;|&gt;CIV&lt;|&gt;CMR&lt;|&gt;COD&lt;|&gt;COG&lt;|&gt;COL&lt;|&gt;COM&lt;|&gt;CPV&lt;|&gt;CRI&lt;|&gt;CYP&lt;|&gt;CZE&lt;|&gt;DEU&lt;|&gt;DJI&lt;|&gt;DMA&lt;|&gt;DNK&lt;|&gt;DOM&lt;|&gt;ECU&lt;|&gt;EGY&lt;|&gt;ESP&lt;|&gt;EST&lt;|&gt;ETH&lt;|&gt;FIN&lt;|&gt;FJI&lt;|&gt;FRA&lt;|&gt;GAB&lt;|&gt;GBR&lt;|&gt;GEO&lt;|&gt;GHA&lt;|&gt;GIN&lt;|&gt;GMB&lt;|&gt;GNB&lt;|&gt;GNQ&lt;|&gt;GRC&lt;|&gt;GRD&lt;|&gt;GTM&lt;|&gt;HKG&lt;|&gt;HND&lt;|&gt;HRV&lt;|&gt;HUN&lt;|&gt;IDN&lt;|&gt;IND&lt;|&gt;IRL&lt;|&gt;IRN&lt;|&gt;IRQ&lt;|&gt;ISL&lt;|&gt;ISR&lt;|&gt;ITA&lt;|&gt;JAM&lt;|&gt;JOR&lt;|&gt;JPN&lt;|&gt;KAZ&lt;|&gt;KEN&lt;|&gt;KGZ&lt;|&gt;KHM&lt;|&gt;KNA&lt;|&gt;KOR&lt;|&gt;KWT&lt;|&gt;LAO&lt;|&gt;LBN&lt;|&gt;LBR&lt;|&gt;LCA&lt;|&gt;LKA&lt;|&gt;LSO&lt;|&gt;LTU&lt;|&gt;LUX&lt;|&gt;LVA&lt;|&gt;MAC&lt;|&gt;MAR&lt;|&gt;MDA&lt;|&gt;MDG&lt;|&gt;MDV&lt;|&gt;MEX&lt;|&gt;MKD&lt;|&gt;MLI&lt;|&gt;MLT&lt;|&gt;MNE&lt;|&gt;MNG&lt;|&gt;MOZ&lt;|&gt;MRT&lt;|&gt;MUS&lt;|&gt;MWI&lt;|&gt;MYS&lt;|&gt;NAM&lt;|&gt;NER&lt;|&gt;NGA&lt;|&gt;NLD&lt;|&gt;NOR&lt;|&gt;NPL&lt;|&gt;NZL&lt;|&gt;OMN&lt;|&gt;PAK&lt;|&gt;PAN&lt;|&gt;PER&lt;|&gt;PHL&lt;|&gt;POL&lt;|&gt;PRT&lt;|&gt;PRY&lt;|&gt;QAT&lt;|&gt;ROU&lt;|&gt;RUS&lt;|&gt;RWA&lt;|&gt;SAU&lt;|&gt;SDN&lt;|&gt;SEN&lt;|&gt;SGP&lt;|&gt;SLE&lt;|&gt;SLV&lt;|&gt;SRB&lt;|&gt;STP&lt;|&gt;SUR&lt;|&gt;SVK&lt;|&gt;SVN&lt;|&gt;SWE&lt;|&gt;SWZ&lt;|&gt;SYR&lt;|&gt;TCD&lt;|&gt;TGO&lt;|&gt;THA&lt;|&gt;TJK&lt;|&gt;TKM&lt;|&gt;TTO&lt;|&gt;TUN&lt;|&gt;TUR&lt;|&gt;TWN&lt;|&gt;TZA&lt;|&gt;UGA&lt;|&gt;UKR&lt;|&gt;URY&lt;|&gt;USA&lt;|&gt;UZB&lt;|&gt;VCT&lt;|&gt;VEN&lt;|&gt;VNM&lt;|&gt;YEM&lt;|&gt;ZAF&lt;|&gt;ZMB&lt;|&gt;ZWE</t>
+  </si>
+  <si>
+    <t>Angola&lt;|&gt;Albania&lt;|&gt;Argentina&lt;|&gt;Armenia&lt;|&gt;Antigua and Barbuda&lt;|&gt;Australia&lt;|&gt;Austria&lt;|&gt;Azerbaijan&lt;|&gt;Burundi&lt;|&gt;Belgium&lt;|&gt;Benin&lt;|&gt;Burkina Faso&lt;|&gt;Bangladesh&lt;|&gt;Bulgaria&lt;|&gt;Bahrain&lt;|&gt;Bahamas&lt;|&gt;Bosnia and Herzegovina&lt;|&gt;Belarus&lt;|&gt;Belize&lt;|&gt;Bermuda&lt;|&gt;Bolivia&lt;|&gt;Brazil&lt;|&gt;Barbados&lt;|&gt;Brunei&lt;|&gt;Bhutan&lt;|&gt;Botswana&lt;|&gt;Central African Republic&lt;|&gt;Canada&lt;|&gt;Switzerland&lt;|&gt;Chile&lt;|&gt;China&lt;|&gt;Cote d'Ivoire&lt;|&gt;Cameroon&lt;|&gt;Congo, Democratic Republic&lt;|&gt;Congo, Republic of&lt;|&gt;Colombia&lt;|&gt;Comoros&lt;|&gt;Cape Verde&lt;|&gt;Costa Rica&lt;|&gt;Cyprus&lt;|&gt;Czech Republic&lt;|&gt;Germany&lt;|&gt;Djibouti&lt;|&gt;Dominica&lt;|&gt;Denmark&lt;|&gt;Dominican Republic&lt;|&gt;Ecuador&lt;|&gt;Egypt&lt;|&gt;Spain&lt;|&gt;Estonia&lt;|&gt;Ethiopia&lt;|&gt;Finland&lt;|&gt;Fiji&lt;|&gt;France&lt;|&gt;Gabon&lt;|&gt;United Kingdom&lt;|&gt;Georgia&lt;|&gt;Ghana&lt;|&gt;Guinea&lt;|&gt;Gambia&lt;|&gt;Guinea-Bissau&lt;|&gt;Equatorial Guinea&lt;|&gt;Greece&lt;|&gt;Grenada&lt;|&gt;Guatemala&lt;|&gt;Hong Kong&lt;|&gt;Honduras&lt;|&gt;Croatia&lt;|&gt;Hungary&lt;|&gt;Indonesia&lt;|&gt;India&lt;|&gt;Ireland&lt;|&gt;Iran&lt;|&gt;Iraq&lt;|&gt;Iceland&lt;|&gt;Israel&lt;|&gt;Italy&lt;|&gt;Jamaica&lt;|&gt;Jordan&lt;|&gt;Japan&lt;|&gt;Kazakhstan&lt;|&gt;Kenya&lt;|&gt;Kyrgyzstan&lt;|&gt;Cambodia&lt;|&gt;St. Kitts &amp; Nevis&lt;|&gt;Korea, Republic of&lt;|&gt;Kuwait&lt;|&gt;Laos&lt;|&gt;Lebanon&lt;|&gt;Liberia&lt;|&gt;St. Lucia&lt;|&gt;Sri Lanka&lt;|&gt;Lesotho&lt;|&gt;Lithuania&lt;|&gt;Luxembourg&lt;|&gt;Latvia&lt;|&gt;Macao&lt;|&gt;Morocco&lt;|&gt;Moldova&lt;|&gt;Madagascar&lt;|&gt;Maldives&lt;|&gt;Mexico&lt;|&gt;Macedonia&lt;|&gt;Mali&lt;|&gt;Malta&lt;|&gt;Montenegro&lt;|&gt;Mongolia&lt;|&gt;Mozambique&lt;|&gt;Mauritania&lt;|&gt;Mauritius&lt;|&gt;Malawi&lt;|&gt;Malaysia&lt;|&gt;Namibia&lt;|&gt;Niger&lt;|&gt;Nigeria&lt;|&gt;Netherlands&lt;|&gt;Norway&lt;|&gt;Nepal&lt;|&gt;New Zealand&lt;|&gt;Oman&lt;|&gt;Pakistan&lt;|&gt;Panama&lt;|&gt;Peru&lt;|&gt;Philippines&lt;|&gt;Poland&lt;|&gt;Portugal&lt;|&gt;Paraguay&lt;|&gt;Qatar&lt;|&gt;Romania&lt;|&gt;Russia&lt;|&gt;Rwanda&lt;|&gt;Saudi Arabia&lt;|&gt;Sudan&lt;|&gt;Senegal&lt;|&gt;Singapore&lt;|&gt;Sierra Leone&lt;|&gt;El Salvador&lt;|&gt;Serbia&lt;|&gt;Sao Tome and Principe&lt;|&gt;Suriname&lt;|&gt;Slovakia&lt;|&gt;Slovenia&lt;|&gt;Sweden&lt;|&gt;Swaziland&lt;|&gt;Syria&lt;|&gt;Chad&lt;|&gt;Togo&lt;|&gt;Thailand&lt;|&gt;Tajikistan&lt;|&gt;Turkmenistan&lt;|&gt;Trinidad &amp; Tobago&lt;|&gt;Tunisia&lt;|&gt;Turkey&lt;|&gt;Taiwan&lt;|&gt;Tanzania&lt;|&gt;Uganda&lt;|&gt;Ukraine&lt;|&gt;Uruguay&lt;|&gt;United States of America&lt;|&gt;Uzbekistan&lt;|&gt;St. Vincent &amp; Grenadines&lt;|&gt;Venezuela&lt;|&gt;Vietnam&lt;|&gt;Yemen&lt;|&gt;South Africa&lt;|&gt;Zambia&lt;|&gt;Zimbabwe</t>
+  </si>
+  <si>
+    <t>LTU&lt;|&gt;URY&lt;|&gt;MEX&lt;|&gt;GAB</t>
+  </si>
+  <si>
+    <t>Lithuania&lt;|&gt;Uruguay&lt;|&gt;Mexico&lt;|&gt;Gabon</t>
+  </si>
+  <si>
+    <t>Dominica&lt;|&gt;Mali&lt;|&gt;Burkina Faso&lt;|&gt;Burundi</t>
+  </si>
+  <si>
+    <t>LTU and DMA&lt;|&gt;URY and MLI&lt;|&gt;MEX and BFA&lt;|&gt;GAB and BDI</t>
+  </si>
+  <si>
+    <t>What are the three-letter country code (ISO 3166-1 alpha-3) for [[1]] and [[2]]?</t>
+  </si>
+  <si>
+    <t>What are the three-letter country code (ISO 3166-1 alpha-3) for {{1}}?</t>
+  </si>
+  <si>
+    <t>a_4</t>
+  </si>
+  <si>
+    <t>St. Vincent &amp; Grenadines&lt;|&gt;Paraguay&lt;|&gt;Belize&lt;|&gt;Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>[[2]], [[3]] and [[4]]</t>
+  </si>
+  <si>
+    <t>2.LTU, 3.DMA, 4.VCT&lt;|&gt;2.URY, 3.MLI, 4.PRY&lt;|&gt;2.MEX, 3.BFA, 4.BLZ&lt;|&gt;2.GAB, 3.BDI, 4.KGZ</t>
+  </si>
+  <si>
+    <t>What are the three-letter country code (ISO 3166-1 alpha-3) for [[1]], {{2}}?</t>
+  </si>
+  <si>
+    <t>[[3]] and [[4]]</t>
+  </si>
+  <si>
+    <t>1.LTU, 3.DMA, 4.VCT&lt;|&gt;1.URY, 3.MLI, 4.PRY&lt;|&gt;1.MEX, 3.BFA, 4.BLZ&lt;|&gt;1.GAB, 3.BDI, 4.KGZ</t>
   </si>
 </sst>
 </file>
@@ -122,9 +161,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12F42F2D-6E43-4E69-B88B-49F8108A5AE1}" name="Tabla1" displayName="Tabla1" ref="A1:H12" totalsRowShown="0">
-  <autoFilter ref="A1:H12" xr:uid="{12F42F2D-6E43-4E69-B88B-49F8108A5AE1}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12F42F2D-6E43-4E69-B88B-49F8108A5AE1}" name="Tabla1" displayName="Tabla1" ref="A1:I9" totalsRowShown="0">
+  <autoFilter ref="A1:I9" xr:uid="{12F42F2D-6E43-4E69-B88B-49F8108A5AE1}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4800CD23-D0A5-4135-9012-8354E0D88484}" name="type"/>
     <tableColumn id="2" xr3:uid="{66BA156C-96AE-4A8A-AEAB-E16828283CF1}" name="question"/>
     <tableColumn id="3" xr3:uid="{076505AD-0808-44F4-891B-0437F91DAFAE}" name="image"/>
@@ -133,6 +172,7 @@
     <tableColumn id="6" xr3:uid="{519C8C4F-468A-4388-B303-858059203502}" name="a_1"/>
     <tableColumn id="7" xr3:uid="{C7ED1195-2EE7-4D03-9F98-681D1299A2E1}" name="a_2"/>
     <tableColumn id="8" xr3:uid="{E25AC271-F30E-40EA-981E-A1B4223CC166}" name="a_3"/>
+    <tableColumn id="9" xr3:uid="{F1EBC332-FAE4-4EE1-8373-C743257E0C62}" name="a_4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,11 +453,12 @@
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="48.140625" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="56" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,16 +483,132 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>